<commit_message>
Update Excel and Word tables
</commit_message>
<xml_diff>
--- a/data/processed/tables.xlsx
+++ b/data/processed/tables.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="prevalenceOverall" sheetId="2" r:id="rId1"/>
-    <sheet name="prevalenceControl" sheetId="5" r:id="rId2"/>
+    <sheet name="prevalenceControl" sheetId="6" r:id="rId2"/>
     <sheet name="prevalenceByExposure" sheetId="3" r:id="rId3"/>
     <sheet name="incidence" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -848,7 +848,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:E24" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E24" totalsRowShown="0">
   <autoFilter ref="A1:E24"/>
   <tableColumns count="5">
     <tableColumn id="1" name="outcomeCategory"/>
@@ -1715,7 +1715,7 @@
         <v>0.41089337050000002</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <v>1.3167973381</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1732,7 +1732,7 @@
         <v>5.2667380000000002E-4</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>0.59131469940000003</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1749,7 +1749,7 @@
         <v>2.7890890737</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
+        <v>9.6489245151999992</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1766,7 +1766,7 @@
         <v>0.78193508739999995</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>2.3395093952999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1783,7 +1783,7 @@
         <v>0.5166670324</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>2.2403606433999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1800,7 +1800,7 @@
         <v>1.0533476700000001E-2</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>0.50945870419999995</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1817,7 +1817,7 @@
         <v>0.1071781255</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>6.4751344796000003</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1834,7 +1834,7 @@
         <v>0.33751014940000001</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>0.71426132009999999</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1851,7 +1851,7 @@
         <v>1.9059448309</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>0.37718808939999998</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1868,7 +1868,7 @@
         <v>1.8541552371000001</v>
       </c>
       <c r="E11" s="1">
-        <v>0</v>
+        <v>0.44446179139999997</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1885,7 +1885,7 @@
         <v>1.6941341700000001E-2</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>1.59917342E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1902,7 +1902,7 @@
         <v>4.8453992799999998E-2</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>0.12609075820000001</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1919,7 +1919,7 @@
         <v>2.2383638000000001E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>7.2965675199999996E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1936,7 +1936,7 @@
         <v>6.9345387999999999E-3</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>9.9745054E-3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1953,7 +1953,7 @@
         <v>2.7211481000000001E-3</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>2.8622493700000001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1970,7 +1970,7 @@
         <v>0.53711953300000004</v>
       </c>
       <c r="E17" s="1">
-        <v>0</v>
+        <v>4.7482440263000001</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1987,7 +1987,7 @@
         <v>4.7400645000000002E-3</v>
       </c>
       <c r="E18" s="1">
-        <v>0</v>
+        <v>1.9461127299999999E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2004,7 +2004,7 @@
         <v>3.71305054E-2</v>
       </c>
       <c r="E19" s="1">
-        <v>0</v>
+        <v>0.14164881830000001</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2021,7 +2021,7 @@
         <v>0.35015032149999997</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>1.3724160475</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2038,7 +2038,7 @@
         <v>0.99506243279999995</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
+        <v>2.7895005320999999</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2055,7 +2055,7 @@
         <v>4.1980293620999998</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>0.37876015810000002</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2072,7 +2072,7 @@
         <v>0.91360354629999996</v>
       </c>
       <c r="E23" s="1">
-        <v>0</v>
+        <v>0.14126935339999999</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2089,7 +2089,7 @@
         <v>0.16230332019999999</v>
       </c>
       <c r="E24" s="1">
-        <v>0</v>
+        <v>0.31891312589999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel and Word documents
Summary of changes
* Fixed denomincator used in overall prevalence calculation
* Fixed filtering of claims to satisfy physician-diagnosed criterion
  * Use enc_type in ("IP", "AV", "ED", "NH", "HH") instead of provider type
* In progress incidence rates are greyed-out
</commit_message>
<xml_diff>
--- a/data/processed/tables.xlsx
+++ b/data/processed/tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="prevalenceOverall" sheetId="2" r:id="rId1"/>
@@ -181,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,6 +312,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -658,7 +665,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -667,6 +674,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -715,17 +725,6 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="27">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -813,6 +812,17 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -853,9 +863,9 @@
   <tableColumns count="5">
     <tableColumn id="1" name="outcomeCategory"/>
     <tableColumn id="2" name="disease"/>
-    <tableColumn id="3" name="timeWindow" dataDxfId="2"/>
-    <tableColumn id="4" name="MPCD Non-AS cohort" dataDxfId="1"/>
-    <tableColumn id="5" name="Medicare Non-AS cohort" dataDxfId="0"/>
+    <tableColumn id="3" name="timeWindow" dataDxfId="22"/>
+    <tableColumn id="4" name="MPCD Non-AS cohort" dataDxfId="21"/>
+    <tableColumn id="5" name="Medicare Non-AS cohort" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -867,36 +877,36 @@
   <tableColumns count="12">
     <tableColumn id="1" name="outcomeCategory"/>
     <tableColumn id="2" name="disease"/>
-    <tableColumn id="3" name="timeWindow" dataDxfId="22"/>
-    <tableColumn id="4" name="MPCD TNF" dataDxfId="21"/>
-    <tableColumn id="5" name="MPCD DMARD" dataDxfId="20"/>
-    <tableColumn id="6" name="MPCD NSAID or no exposure" dataDxfId="19"/>
-    <tableColumn id="7" name="Marketscan TNF" dataDxfId="18"/>
-    <tableColumn id="8" name="Marketscan DMARD" dataDxfId="17"/>
-    <tableColumn id="9" name="Marketscan NSAID or no exposure" dataDxfId="16"/>
-    <tableColumn id="10" name="Medicare TNF" dataDxfId="15"/>
-    <tableColumn id="11" name="Medicare DMARD" dataDxfId="14"/>
-    <tableColumn id="12" name="Medicare NSAID or no exposure" dataDxfId="13"/>
+    <tableColumn id="3" name="timeWindow" dataDxfId="19"/>
+    <tableColumn id="4" name="MPCD TNF" dataDxfId="18"/>
+    <tableColumn id="5" name="MPCD DMARD" dataDxfId="17"/>
+    <tableColumn id="6" name="MPCD NSAID or no exposure" dataDxfId="16"/>
+    <tableColumn id="7" name="Marketscan TNF" dataDxfId="15"/>
+    <tableColumn id="8" name="Marketscan DMARD" dataDxfId="14"/>
+    <tableColumn id="9" name="Marketscan NSAID or no exposure" dataDxfId="13"/>
+    <tableColumn id="10" name="Medicare TNF" dataDxfId="12"/>
+    <tableColumn id="11" name="Medicare DMARD" dataDxfId="11"/>
+    <tableColumn id="12" name="Medicare NSAID or no exposure" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K24" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K24" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:K24"/>
   <tableColumns count="11">
     <tableColumn id="1" name="outcomeCategory"/>
     <tableColumn id="2" name="disease"/>
-    <tableColumn id="3" name="MPCD TNF" dataDxfId="11"/>
-    <tableColumn id="4" name="MPCD DMARD" dataDxfId="10"/>
-    <tableColumn id="5" name="MPCD NSAID or no exposure" dataDxfId="9"/>
-    <tableColumn id="6" name="Marketscan TNF" dataDxfId="8"/>
-    <tableColumn id="7" name="Marketscan DMARD" dataDxfId="7"/>
-    <tableColumn id="8" name="Marketscan NSAID or no exposure" dataDxfId="6"/>
-    <tableColumn id="9" name="Medicare TNF" dataDxfId="5"/>
-    <tableColumn id="10" name="Medicare DMARD" dataDxfId="4"/>
-    <tableColumn id="11" name="Medicare NSAID or no exposure" dataDxfId="3"/>
+    <tableColumn id="3" name="MPCD TNF" dataDxfId="8"/>
+    <tableColumn id="4" name="MPCD DMARD" dataDxfId="7"/>
+    <tableColumn id="5" name="MPCD NSAID or no exposure" dataDxfId="6"/>
+    <tableColumn id="6" name="Marketscan TNF" dataDxfId="5"/>
+    <tableColumn id="7" name="Marketscan DMARD" dataDxfId="4"/>
+    <tableColumn id="8" name="Marketscan NSAID or no exposure" dataDxfId="3"/>
+    <tableColumn id="9" name="Medicare TNF" dataDxfId="2"/>
+    <tableColumn id="10" name="Medicare DMARD" dataDxfId="1"/>
+    <tableColumn id="11" name="Medicare NSAID or no exposure" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1168,7 +1178,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,13 +1222,13 @@
         <v>14</v>
       </c>
       <c r="D2" s="1">
-        <v>0.34458993799999998</v>
+        <v>0.53333333329999999</v>
       </c>
       <c r="E2" s="1">
-        <v>0.38016618689999998</v>
+        <v>0.56751794359999996</v>
       </c>
       <c r="F2" s="1">
-        <v>1.8660723875</v>
+        <v>1.5674814027999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1235,10 +1245,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>0.195514039</v>
+        <v>0.62593890839999999</v>
       </c>
       <c r="F3" s="1">
-        <v>1.337128128</v>
+        <v>1.8552957846</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1252,13 +1262,13 @@
         <v>14</v>
       </c>
       <c r="D4" s="1">
-        <v>2.8486101539000002</v>
+        <v>4</v>
       </c>
       <c r="E4" s="1">
-        <v>2.0094498451999998</v>
+        <v>3.4885661826000001</v>
       </c>
       <c r="F4" s="1">
-        <v>10.7856299</v>
+        <v>9.7591215018999993</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1272,13 +1282,13 @@
         <v>14</v>
       </c>
       <c r="D5" s="1">
-        <v>1.5621410521000001</v>
+        <v>1.9</v>
       </c>
       <c r="E5" s="1">
-        <v>0.65171346330000002</v>
+        <v>1.3269904857000001</v>
       </c>
       <c r="F5" s="1">
-        <v>4.0355493502000002</v>
+        <v>4.8662770103000001</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1292,13 +1302,13 @@
         <v>14</v>
       </c>
       <c r="D6" s="1">
-        <v>0.45945325059999997</v>
+        <v>0.63333333329999997</v>
       </c>
       <c r="E6" s="1">
-        <v>0.76576331939999998</v>
+        <v>1.2602236687999999</v>
       </c>
       <c r="F6" s="1">
-        <v>3.9147245194</v>
+        <v>4.5120439249000004</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1312,13 +1322,13 @@
         <v>14</v>
       </c>
       <c r="D7" s="1">
-        <v>2.2972662500000001E-2</v>
+        <v>0.46666666670000001</v>
       </c>
       <c r="E7" s="1">
-        <v>0.391028078</v>
+        <v>0.58420964779999995</v>
       </c>
       <c r="F7" s="1">
-        <v>0.8457738159</v>
+        <v>1.7888770811000001</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1332,13 +1342,13 @@
         <v>14</v>
       </c>
       <c r="D8" s="1">
-        <v>0.13783597519999999</v>
+        <v>5.2</v>
       </c>
       <c r="E8" s="1">
-        <v>4.518546679</v>
+        <v>6.8936738441000003</v>
       </c>
       <c r="F8" s="1">
-        <v>13.513586081</v>
+        <v>19.416400992</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1352,13 +1362,13 @@
         <v>14</v>
       </c>
       <c r="D9" s="1">
-        <v>0.98782448889999996</v>
+        <v>1.0666666667</v>
       </c>
       <c r="E9" s="1">
-        <v>0.63542062669999999</v>
+        <v>1.0181939576000001</v>
       </c>
       <c r="F9" s="1">
-        <v>2.4487165717999999</v>
+        <v>2.4442082891000001</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1372,13 +1382,13 @@
         <v>14</v>
       </c>
       <c r="D10" s="1">
-        <v>3.9742706179999998</v>
+        <v>4.2666666666999999</v>
       </c>
       <c r="E10" s="1">
-        <v>2.5579753434999999</v>
+        <v>3.5720247036999999</v>
       </c>
       <c r="F10" s="1">
-        <v>5.0558479217999999</v>
+        <v>4.7954303932000002</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1392,13 +1402,13 @@
         <v>14</v>
       </c>
       <c r="D11" s="1">
-        <v>2.0905122904</v>
+        <v>2.4666666667000001</v>
       </c>
       <c r="E11" s="1">
-        <v>1.4935100201</v>
+        <v>2.6122517108999999</v>
       </c>
       <c r="F11" s="1">
-        <v>2.7977660831</v>
+        <v>2.6656039674000001</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1412,13 +1422,13 @@
         <v>14</v>
       </c>
       <c r="D12" s="1">
-        <v>2.2972662500000001E-2</v>
+        <v>3.3333333299999997E-2</v>
       </c>
       <c r="E12" s="1">
-        <v>5.4309455000000001E-3</v>
+        <v>2.50375563E-2</v>
       </c>
       <c r="F12" s="1">
-        <v>8.0549887200000003E-2</v>
+        <v>7.0846617099999995E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1432,13 +1442,13 @@
         <v>14</v>
       </c>
       <c r="D13" s="1">
-        <v>0.18378130030000001</v>
+        <v>0.1</v>
       </c>
       <c r="E13" s="1">
-        <v>3.8016618699999997E-2</v>
+        <v>0.14187948589999999</v>
       </c>
       <c r="F13" s="1">
-        <v>0.2282246805</v>
+        <v>0.22582359190000001</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1455,10 +1465,10 @@
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>1.08618911E-2</v>
+        <v>1.6691704200000001E-2</v>
       </c>
       <c r="F14" s="1">
-        <v>0.1933197294</v>
+        <v>0.15054906130000001</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1475,10 +1485,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>5.4309455000000001E-3</v>
+        <v>1.6691704200000001E-2</v>
       </c>
       <c r="F15" s="1">
-        <v>2.9534958699999999E-2</v>
+        <v>1.3283740699999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1492,13 +1502,13 @@
         <v>14</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>6.6666666700000002E-2</v>
       </c>
       <c r="E16" s="1">
-        <v>5.9740400800000003E-2</v>
+        <v>0.11684192960000001</v>
       </c>
       <c r="F16" s="1">
-        <v>0.46181935349999997</v>
+        <v>0.65533120789999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1512,13 +1522,13 @@
         <v>14</v>
       </c>
       <c r="D17" s="1">
-        <v>0.96485182629999999</v>
+        <v>1.2666666666999999</v>
       </c>
       <c r="E17" s="1">
-        <v>0.90153695759999997</v>
+        <v>1.3520280420999999</v>
       </c>
       <c r="F17" s="1">
-        <v>9.1316722157000001</v>
+        <v>3.1925256818999999</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1532,13 +1542,13 @@
         <v>14</v>
       </c>
       <c r="D18" s="1">
-        <v>4.5945325100000003E-2</v>
+        <v>0.1333333333</v>
       </c>
       <c r="E18" s="1">
-        <v>2.7154727600000001E-2</v>
+        <v>5.00751127E-2</v>
       </c>
       <c r="F18" s="1">
-        <v>0.16109977449999999</v>
+        <v>0.2081119377</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1552,13 +1562,13 @@
         <v>14</v>
       </c>
       <c r="D19" s="1">
-        <v>0.25269928780000001</v>
+        <v>0.16666666669999999</v>
       </c>
       <c r="E19" s="1">
-        <v>0.1792212024</v>
+        <v>0.2420297112</v>
       </c>
       <c r="F19" s="1">
-        <v>1.0337235527999999</v>
+        <v>0.85015940489999997</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1572,13 +1582,13 @@
         <v>14</v>
       </c>
       <c r="D20" s="1">
-        <v>1.7229496899000001</v>
+        <v>2.4</v>
       </c>
       <c r="E20" s="1">
-        <v>1.4500624558999999</v>
+        <v>2.2450342179999998</v>
       </c>
       <c r="F20" s="1">
-        <v>6.7447105574000004</v>
+        <v>7.3193411265000003</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1592,13 +1602,13 @@
         <v>14</v>
       </c>
       <c r="D21" s="1">
-        <v>2.2513209281000002</v>
+        <v>2.9333333332999998</v>
       </c>
       <c r="E21" s="1">
-        <v>1.5043719111</v>
+        <v>1.8527791687999999</v>
       </c>
       <c r="F21" s="1">
-        <v>4.5993985608000001</v>
+        <v>4.4854764434999996</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1612,13 +1622,13 @@
         <v>14</v>
       </c>
       <c r="D22" s="1">
-        <v>2.4351022282999999</v>
+        <v>2.5</v>
       </c>
       <c r="E22" s="1">
-        <v>0.65171346330000002</v>
+        <v>2.7040560840999999</v>
       </c>
       <c r="F22" s="1">
-        <v>2.5319514553000002</v>
+        <v>3.7902940135000001</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1632,13 +1642,13 @@
         <v>14</v>
       </c>
       <c r="D23" s="1">
-        <v>3.8134619802</v>
+        <v>3.6666666666999999</v>
       </c>
       <c r="E23" s="1">
-        <v>1.2871340899999999</v>
+        <v>4.0560841262</v>
       </c>
       <c r="F23" s="1">
-        <v>5.1686177639000004</v>
+        <v>4.9902585901999998</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1652,13 +1662,13 @@
         <v>14</v>
       </c>
       <c r="D24" s="1">
-        <v>5.8350562830000001</v>
+        <v>7.0333333332999999</v>
       </c>
       <c r="E24" s="1">
-        <v>1.6564383859</v>
+        <v>7.5863795694</v>
       </c>
       <c r="F24" s="1">
-        <v>4.9108581247999998</v>
+        <v>4.0161176053999998</v>
       </c>
     </row>
   </sheetData>
@@ -1673,7 +1683,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1712,10 +1724,10 @@
         <v>14</v>
       </c>
       <c r="D2" s="1">
-        <v>0.41089337050000002</v>
+        <v>0.58109679830000005</v>
       </c>
       <c r="E2" s="1">
-        <v>1.3167973381</v>
+        <v>1.1851230252</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1732,7 +1744,7 @@
         <v>5.2667380000000002E-4</v>
       </c>
       <c r="E3" s="1">
-        <v>0.59131469940000003</v>
+        <v>0.74158279140000005</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1746,10 +1758,10 @@
         <v>14</v>
       </c>
       <c r="D4" s="1">
-        <v>2.7890890737</v>
+        <v>3.8708771313999999</v>
       </c>
       <c r="E4" s="1">
-        <v>9.6489245151999992</v>
+        <v>8.8094939944000004</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1763,10 +1775,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="1">
-        <v>0.78193508739999995</v>
+        <v>0.88437314840000003</v>
       </c>
       <c r="E5" s="1">
-        <v>2.3395093952999999</v>
+        <v>2.6727337680000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1780,10 +1792,10 @@
         <v>14</v>
       </c>
       <c r="D6" s="1">
-        <v>0.5166670324</v>
+        <v>0.67300138249999997</v>
       </c>
       <c r="E6" s="1">
-        <v>2.2403606433999999</v>
+        <v>2.2508230322</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1797,10 +1809,10 @@
         <v>14</v>
       </c>
       <c r="D7" s="1">
-        <v>1.0533476700000001E-2</v>
+        <v>0.22181746359999999</v>
       </c>
       <c r="E7" s="1">
-        <v>0.50945870419999995</v>
+        <v>0.99913102539999998</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1814,10 +1826,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="1">
-        <v>0.1071781255</v>
+        <v>2.2366082205</v>
       </c>
       <c r="E8" s="1">
-        <v>6.4751344796000003</v>
+        <v>8.8800744618999996</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1831,10 +1843,10 @@
         <v>14</v>
       </c>
       <c r="D9" s="1">
-        <v>0.33751014940000001</v>
+        <v>0.41958348880000002</v>
       </c>
       <c r="E9" s="1">
-        <v>0.71426132009999999</v>
+        <v>0.85737378860000002</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1848,10 +1860,10 @@
         <v>14</v>
       </c>
       <c r="D10" s="1">
-        <v>1.9059448309</v>
+        <v>2.1527793016999999</v>
       </c>
       <c r="E10" s="1">
-        <v>0.37718808939999998</v>
+        <v>0.34303625030000001</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1865,10 +1877,10 @@
         <v>14</v>
       </c>
       <c r="D11" s="1">
-        <v>1.8541552371000001</v>
+        <v>2.0025894797000001</v>
       </c>
       <c r="E11" s="1">
-        <v>0.44446179139999997</v>
+        <v>0.37480288150000002</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1882,10 +1894,10 @@
         <v>14</v>
       </c>
       <c r="D12" s="1">
-        <v>1.6941341700000001E-2</v>
+        <v>2.1944743100000001E-2</v>
       </c>
       <c r="E12" s="1">
-        <v>1.59917342E-2</v>
+        <v>1.3064433699999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1899,10 +1911,10 @@
         <v>14</v>
       </c>
       <c r="D13" s="1">
-        <v>4.8453992799999998E-2</v>
+        <v>7.5314358400000003E-2</v>
       </c>
       <c r="E13" s="1">
-        <v>0.12609075820000001</v>
+        <v>0.1033770748</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1916,10 +1928,10 @@
         <v>14</v>
       </c>
       <c r="D14" s="1">
-        <v>2.2383638000000001E-2</v>
+        <v>4.3011696500000002E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>7.2965675199999996E-2</v>
+        <v>6.02264972E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1933,10 +1945,10 @@
         <v>14</v>
       </c>
       <c r="D15" s="1">
-        <v>6.9345387999999999E-3</v>
+        <v>7.7245496E-3</v>
       </c>
       <c r="E15" s="1">
-        <v>9.9745054E-3</v>
+        <v>8.1855994999999997E-3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1950,10 +1962,10 @@
         <v>14</v>
       </c>
       <c r="D16" s="1">
-        <v>2.7211481000000001E-3</v>
+        <v>1.67657838E-2</v>
       </c>
       <c r="E16" s="1">
-        <v>2.8622493700000001E-2</v>
+        <v>4.16327181E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1967,10 +1979,10 @@
         <v>14</v>
       </c>
       <c r="D17" s="1">
-        <v>0.53711953300000004</v>
+        <v>0.65123219730000004</v>
       </c>
       <c r="E17" s="1">
-        <v>4.7482440263000001</v>
+        <v>1.2652443239</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1984,10 +1996,10 @@
         <v>14</v>
       </c>
       <c r="D18" s="1">
-        <v>4.7400645000000002E-3</v>
+        <v>6.9345387999999999E-3</v>
       </c>
       <c r="E18" s="1">
-        <v>1.9461127299999999E-2</v>
+        <v>1.8160104900000001E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2001,10 +2013,10 @@
         <v>14</v>
       </c>
       <c r="D19" s="1">
-        <v>3.71305054E-2</v>
+        <v>3.9061642799999997E-2</v>
       </c>
       <c r="E19" s="1">
-        <v>0.14164881830000001</v>
+        <v>8.2289669400000001E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2018,10 +2030,10 @@
         <v>14</v>
       </c>
       <c r="D20" s="1">
-        <v>0.35015032149999997</v>
+        <v>0.4532906142</v>
       </c>
       <c r="E20" s="1">
-        <v>1.3724160475</v>
+        <v>1.1173614398</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2035,10 +2047,10 @@
         <v>14</v>
       </c>
       <c r="D21" s="1">
-        <v>0.99506243279999995</v>
+        <v>1.1884395093</v>
       </c>
       <c r="E21" s="1">
-        <v>2.7895005320999999</v>
+        <v>2.5481066600000002</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2052,10 +2064,10 @@
         <v>14</v>
       </c>
       <c r="D22" s="1">
-        <v>4.1980293620999998</v>
+        <v>4.6324474972000003</v>
       </c>
       <c r="E22" s="1">
-        <v>0.37876015810000002</v>
+        <v>0.97132167079999998</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2069,10 +2081,10 @@
         <v>14</v>
       </c>
       <c r="D23" s="1">
-        <v>0.91360354629999996</v>
+        <v>1.0316662643000001</v>
       </c>
       <c r="E23" s="1">
-        <v>0.14126935339999999</v>
+        <v>0.1586163193</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2086,10 +2098,10 @@
         <v>14</v>
       </c>
       <c r="D24" s="1">
-        <v>0.16230332019999999</v>
+        <v>0.21804296779999999</v>
       </c>
       <c r="E24" s="1">
-        <v>0.31891312589999998</v>
+        <v>0.23266617989999999</v>
       </c>
     </row>
   </sheetData>
@@ -2177,25 +2189,25 @@
         <v>0.20790020789999999</v>
       </c>
       <c r="F2" s="1">
-        <v>0.38565368300000002</v>
+        <v>0.50134978789999995</v>
       </c>
       <c r="G2" s="1">
-        <v>0.1557362866</v>
+        <v>0.13843225470000001</v>
       </c>
       <c r="H2" s="1">
-        <v>0.58679706600000003</v>
+        <v>0.78239608800000005</v>
       </c>
       <c r="I2" s="1">
-        <v>0.46274435739999997</v>
+        <v>0.61384455569999996</v>
       </c>
       <c r="J2" s="1">
-        <v>0.79271377970000001</v>
+        <v>0.43852251640000001</v>
       </c>
       <c r="K2" s="1">
-        <v>2.0219526284999998</v>
+        <v>1.6368187944999999</v>
       </c>
       <c r="L2" s="1">
-        <v>2.0787076028000002</v>
+        <v>1.7418268126000001</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2218,22 +2230,22 @@
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>0.2076483821</v>
+        <v>0.51912095520000001</v>
       </c>
       <c r="H3" s="1">
-        <v>0.14669926650000001</v>
+        <v>0.48899755499999997</v>
       </c>
       <c r="I3" s="1">
-        <v>0.19831901029999999</v>
+        <v>0.80271980359999995</v>
       </c>
       <c r="J3" s="1">
-        <v>0.9445100354</v>
+        <v>1.2143700454999999</v>
       </c>
       <c r="K3" s="1">
-        <v>0.94357789329999997</v>
+        <v>1.2901983439</v>
       </c>
       <c r="L3" s="1">
-        <v>1.5044789832000001</v>
+        <v>2.2012097083</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2247,31 +2259,31 @@
         <v>14</v>
       </c>
       <c r="D4" s="1">
-        <v>2.1110242377000001</v>
+        <v>2.5801407349000001</v>
       </c>
       <c r="E4" s="1">
         <v>1.4553014553000001</v>
       </c>
       <c r="F4" s="1">
-        <v>3.4708831468999999</v>
+        <v>4.2421905128999997</v>
       </c>
       <c r="G4" s="1">
-        <v>0.76137740089999995</v>
+        <v>1.7823152794999999</v>
       </c>
       <c r="H4" s="1">
-        <v>2.8850855746000001</v>
+        <v>4.1564792176000003</v>
       </c>
       <c r="I4" s="1">
-        <v>2.5214845594000002</v>
+        <v>4.0041552554999997</v>
       </c>
       <c r="J4" s="1">
-        <v>6.6115702478999996</v>
+        <v>5.7007927138000003</v>
       </c>
       <c r="K4" s="1">
-        <v>8.9543616407000002</v>
+        <v>7.6834199883999998</v>
       </c>
       <c r="L4" s="1">
-        <v>12.097082919</v>
+        <v>10.539009264000001</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2285,31 +2297,31 @@
         <v>14</v>
       </c>
       <c r="D5" s="1">
-        <v>1.7982799061999999</v>
+        <v>1.7200938233</v>
       </c>
       <c r="E5" s="1">
-        <v>1.0395010394999999</v>
+        <v>0.62370062370000001</v>
       </c>
       <c r="F5" s="1">
-        <v>1.5426147320000001</v>
+        <v>1.5811801002999999</v>
       </c>
       <c r="G5" s="1">
-        <v>0.51912095520000001</v>
+        <v>0.81328949650000004</v>
       </c>
       <c r="H5" s="1">
-        <v>0.63569682149999995</v>
+        <v>0.880195599</v>
       </c>
       <c r="I5" s="1">
-        <v>0.72716970439999995</v>
+        <v>1.3315704977</v>
       </c>
       <c r="J5" s="1">
-        <v>2.4793388429999998</v>
+        <v>2.9347276100999999</v>
       </c>
       <c r="K5" s="1">
-        <v>3.3891777393</v>
+        <v>3.6972848064999999</v>
       </c>
       <c r="L5" s="1">
-        <v>4.5172651405000002</v>
+        <v>4.9536788914000001</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2329,25 +2341,25 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>0.65561126110000001</v>
+        <v>0.88700347089999998</v>
       </c>
       <c r="G6" s="1">
-        <v>0.50181692330000005</v>
+        <v>0.70946530539999997</v>
       </c>
       <c r="H6" s="1">
-        <v>0.92909535450000003</v>
+        <v>1.1246943764999999</v>
       </c>
       <c r="I6" s="1">
-        <v>0.87826990270000005</v>
+        <v>1.4637831712</v>
       </c>
       <c r="J6" s="1">
-        <v>2.158880081</v>
+        <v>2.4456063417</v>
       </c>
       <c r="K6" s="1">
-        <v>2.8114769882999999</v>
+        <v>2.9847872136000002</v>
       </c>
       <c r="L6" s="1">
-        <v>4.5325779037</v>
+        <v>4.6091417196000002</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2361,31 +2373,31 @@
         <v>14</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>0.31274433149999997</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
       </c>
       <c r="F7" s="1">
-        <v>3.85653683E-2</v>
+        <v>0.50134978789999995</v>
       </c>
       <c r="G7" s="1">
-        <v>0.1557362866</v>
+        <v>0.19034435020000001</v>
       </c>
       <c r="H7" s="1">
-        <v>9.7799511000000006E-2</v>
+        <v>0.14669926650000001</v>
       </c>
       <c r="I7" s="1">
-        <v>0.57606950609999996</v>
+        <v>0.66106336759999995</v>
       </c>
       <c r="J7" s="1">
-        <v>0.26986001009999999</v>
+        <v>0.48912126830000002</v>
       </c>
       <c r="K7" s="1">
-        <v>0.59695744269999995</v>
+        <v>0.90506450989999998</v>
       </c>
       <c r="L7" s="1">
-        <v>1.0259551335999999</v>
+        <v>1.6767475691</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2399,31 +2411,31 @@
         <v>14</v>
       </c>
       <c r="D8" s="1">
-        <v>7.8186082899999995E-2</v>
+        <v>1.0164190773999999</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>1.2474012474</v>
       </c>
       <c r="F8" s="1">
-        <v>0.19282684150000001</v>
+        <v>5.5919784033999997</v>
       </c>
       <c r="G8" s="1">
-        <v>2.9070773490000001</v>
+        <v>3.5300224951999999</v>
       </c>
       <c r="H8" s="1">
-        <v>3.4718826406000001</v>
+        <v>4.8410757946</v>
       </c>
       <c r="I8" s="1">
-        <v>5.6001511001999997</v>
+        <v>7.1678156578000003</v>
       </c>
       <c r="J8" s="1">
-        <v>7.1850227693999997</v>
+        <v>9.1415078427999994</v>
       </c>
       <c r="K8" s="1">
-        <v>11.226651261000001</v>
+        <v>13.807047948999999</v>
       </c>
       <c r="L8" s="1">
-        <v>15.404639767000001</v>
+        <v>19.018451880000001</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2446,22 +2458,22 @@
         <v>0.80987273429999995</v>
       </c>
       <c r="G9" s="1">
-        <v>0.74407336909999999</v>
+        <v>1.1766741650999999</v>
       </c>
       <c r="H9" s="1">
-        <v>0.78239608800000005</v>
+        <v>1.5158924204999999</v>
       </c>
       <c r="I9" s="1">
-        <v>0.54773821889999996</v>
+        <v>0.95382000190000005</v>
       </c>
       <c r="J9" s="1">
-        <v>3.3057851239999998</v>
+        <v>2.7154663518</v>
       </c>
       <c r="K9" s="1">
-        <v>3.1388407472000002</v>
+        <v>2.7729636049000002</v>
       </c>
       <c r="L9" s="1">
-        <v>2.1169895107999999</v>
+        <v>2.2662889518</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2478,28 +2490,28 @@
         <v>5.7857701328999998</v>
       </c>
       <c r="E10" s="1">
-        <v>3.7422037422000001</v>
+        <v>3.9501039500999999</v>
       </c>
       <c r="F10" s="1">
-        <v>3.1237948322000002</v>
+        <v>3.3937524102999999</v>
       </c>
       <c r="G10" s="1">
-        <v>3.7030628135999999</v>
+        <v>5.5372901886000001</v>
       </c>
       <c r="H10" s="1">
-        <v>2.6894865526</v>
+        <v>3.8630806845999999</v>
       </c>
       <c r="I10" s="1">
-        <v>1.9076400038000001</v>
+        <v>2.6820285201999998</v>
       </c>
       <c r="J10" s="1">
-        <v>8.3656603136999994</v>
+        <v>8.3825265643000009</v>
       </c>
       <c r="K10" s="1">
-        <v>6.4124783362000004</v>
+        <v>6.5857885615000002</v>
       </c>
       <c r="L10" s="1">
-        <v>4.0349131000999998</v>
+        <v>3.9162391853999998</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2513,31 +2525,31 @@
         <v>14</v>
       </c>
       <c r="D11" s="1">
-        <v>2.8928850664999999</v>
+        <v>3.0492572322</v>
       </c>
       <c r="E11" s="1">
-        <v>2.4948024948</v>
+        <v>2.2869022869000002</v>
       </c>
       <c r="F11" s="1">
-        <v>1.6197454685999999</v>
+        <v>1.8511376784</v>
       </c>
       <c r="G11" s="1">
-        <v>2.1803080117999998</v>
+        <v>3.6165426543999999</v>
       </c>
       <c r="H11" s="1">
-        <v>1.5158924204999999</v>
+        <v>2.5916870416000002</v>
       </c>
       <c r="I11" s="1">
-        <v>1.1143639625999999</v>
+        <v>2.1059590141000002</v>
       </c>
       <c r="J11" s="1">
-        <v>4.1659639062</v>
+        <v>3.8623713947999998</v>
       </c>
       <c r="K11" s="1">
-        <v>3.8128249567000001</v>
+        <v>3.601001348</v>
       </c>
       <c r="L11" s="1">
-        <v>2.2854299058</v>
+        <v>2.1093331291999999</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2560,22 +2572,22 @@
         <v>3.85653683E-2</v>
       </c>
       <c r="G12" s="1">
-        <v>0</v>
+        <v>3.4608063699999997E-2</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12" s="1">
-        <v>9.4437623999999998E-3</v>
+        <v>2.8331287199999999E-2</v>
       </c>
       <c r="J12" s="1">
         <v>0.1011975038</v>
       </c>
       <c r="K12" s="1">
-        <v>1.9256691699999998E-2</v>
+        <v>3.8513383399999997E-2</v>
       </c>
       <c r="L12" s="1">
-        <v>8.8048388300000002E-2</v>
+        <v>7.2735625100000006E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2595,25 +2607,25 @@
         <v>0.20790020789999999</v>
       </c>
       <c r="F13" s="1">
-        <v>0.1156961049</v>
+        <v>3.85653683E-2</v>
       </c>
       <c r="G13" s="1">
-        <v>5.1912095499999998E-2</v>
+        <v>0.1211282229</v>
       </c>
       <c r="H13" s="1">
-        <v>9.7799511000000006E-2</v>
+        <v>4.8899755500000003E-2</v>
       </c>
       <c r="I13" s="1">
-        <v>1.88875248E-2</v>
+        <v>9.4437623900000003E-2</v>
       </c>
       <c r="J13" s="1">
-        <v>0.18552875699999999</v>
+        <v>0.1180637544</v>
       </c>
       <c r="K13" s="1">
-        <v>0.25033699209999999</v>
+        <v>0.192566917</v>
       </c>
       <c r="L13" s="1">
-        <v>0.2335196386</v>
+        <v>0.18758134909999999</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2627,31 +2639,31 @@
         <v>14</v>
       </c>
       <c r="D14" s="1">
-        <v>0</v>
+        <v>0.15637216579999999</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>0.20790020789999999</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
+        <v>6.9216127399999994E-2</v>
       </c>
       <c r="H14" s="1">
-        <v>0</v>
+        <v>4.8899755500000003E-2</v>
       </c>
       <c r="I14" s="1">
         <v>1.88875248E-2</v>
       </c>
       <c r="J14" s="1">
-        <v>0.18552875699999999</v>
+        <v>0.20239500760000001</v>
       </c>
       <c r="K14" s="1">
-        <v>0.25033699209999999</v>
+        <v>0.23108030039999999</v>
       </c>
       <c r="L14" s="1">
-        <v>0.1837531583</v>
+        <v>0.16461220430000001</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2674,22 +2686,22 @@
         <v>0</v>
       </c>
       <c r="G15" s="1">
-        <v>0</v>
+        <v>1.7304031800000001E-2</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="I15" s="1">
-        <v>9.4437623999999998E-3</v>
+        <v>1.88875248E-2</v>
       </c>
       <c r="J15" s="1">
         <v>0</v>
       </c>
       <c r="K15" s="1">
-        <v>5.7770075099999998E-2</v>
+        <v>3.8513383399999997E-2</v>
       </c>
       <c r="L15" s="1">
-        <v>3.0625526399999999E-2</v>
+        <v>1.9140954000000002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2709,25 +2721,25 @@
         <v>0</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>7.7130736599999999E-2</v>
       </c>
       <c r="G16" s="1">
-        <v>6.9216127399999994E-2</v>
+        <v>0.103824191</v>
       </c>
       <c r="H16" s="1">
-        <v>4.8899755500000003E-2</v>
+        <v>0.14669926650000001</v>
       </c>
       <c r="I16" s="1">
-        <v>5.6662574399999999E-2</v>
+        <v>0.1038813863</v>
       </c>
       <c r="J16" s="1">
-        <v>0.28672626080000002</v>
+        <v>0.43852251640000001</v>
       </c>
       <c r="K16" s="1">
-        <v>0.8280377431</v>
+        <v>1.0783747351999999</v>
       </c>
       <c r="L16" s="1">
-        <v>0.42875736930000002</v>
+        <v>0.62016690910000005</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2747,25 +2759,25 @@
         <v>0.41580041579999999</v>
       </c>
       <c r="F17" s="1">
-        <v>1.1955264173</v>
+        <v>1.5426147320000001</v>
       </c>
       <c r="G17" s="1">
-        <v>0.67485724170000005</v>
+        <v>0.86520159200000002</v>
       </c>
       <c r="H17" s="1">
-        <v>0.83129584349999996</v>
+        <v>0.73349633250000001</v>
       </c>
       <c r="I17" s="1">
-        <v>1.0388138633999999</v>
+        <v>1.3315704977</v>
       </c>
       <c r="J17" s="1">
-        <v>6.5441052453999999</v>
+        <v>2.4456063417</v>
       </c>
       <c r="K17" s="1">
-        <v>9.3972655498000002</v>
+        <v>3.3891777393</v>
       </c>
       <c r="L17" s="1">
-        <v>9.6661817625000008</v>
+        <v>3.0931781639999998</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2785,16 +2797,16 @@
         <v>0</v>
       </c>
       <c r="F18" s="1">
-        <v>7.7130736599999999E-2</v>
+        <v>0.1542614732</v>
       </c>
       <c r="G18" s="1">
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>9.7799511000000006E-2</v>
+        <v>0.14669926650000001</v>
       </c>
       <c r="I18" s="1">
-        <v>2.8331287199999999E-2</v>
+        <v>3.7775049599999999E-2</v>
       </c>
       <c r="J18" s="1">
         <v>0.1349300051</v>
@@ -2803,7 +2815,7 @@
         <v>1.9256691699999998E-2</v>
       </c>
       <c r="L18" s="1">
-        <v>0.19523773059999999</v>
+        <v>0.17226858589999999</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2823,25 +2835,25 @@
         <v>0</v>
       </c>
       <c r="F19" s="1">
-        <v>0.34708831470000001</v>
+        <v>0.2313922098</v>
       </c>
       <c r="G19" s="1">
-        <v>8.6520159200000002E-2</v>
+        <v>0.1557362866</v>
       </c>
       <c r="H19" s="1">
-        <v>0.24449877749999999</v>
+        <v>0.19559902200000001</v>
       </c>
       <c r="I19" s="1">
-        <v>0.21720653509999999</v>
+        <v>0.42496930779999997</v>
       </c>
       <c r="J19" s="1">
-        <v>0.50598751900000005</v>
+        <v>0.25299375950000003</v>
       </c>
       <c r="K19" s="1">
-        <v>0.69324090120000004</v>
+        <v>0.4043905257</v>
       </c>
       <c r="L19" s="1">
-        <v>1.2211928643000001</v>
+        <v>0.74649720539999997</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2855,31 +2867,31 @@
         <v>14</v>
       </c>
       <c r="D20" s="1">
-        <v>1.2509773259999999</v>
+        <v>1.3291634089</v>
       </c>
       <c r="E20" s="1">
-        <v>0.20790020789999999</v>
+        <v>0.41580041579999999</v>
       </c>
       <c r="F20" s="1">
-        <v>2.2367913613999999</v>
+        <v>2.6610104126</v>
       </c>
       <c r="G20" s="1">
-        <v>0.43260079600000001</v>
+        <v>0.57103305069999999</v>
       </c>
       <c r="H20" s="1">
-        <v>0.880195599</v>
+        <v>0.83129584349999996</v>
       </c>
       <c r="I20" s="1">
-        <v>2.1154027764999999</v>
+        <v>2.7103598073000001</v>
       </c>
       <c r="J20" s="1">
-        <v>3.0021926126</v>
+        <v>1.8384213189</v>
       </c>
       <c r="K20" s="1">
-        <v>4.0053918736999998</v>
+        <v>2.6766801463999998</v>
       </c>
       <c r="L20" s="1">
-        <v>8.1387336344999994</v>
+        <v>7.0630120205000004</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2893,31 +2905,31 @@
         <v>14</v>
       </c>
       <c r="D21" s="1">
-        <v>1.7982799061999999</v>
+        <v>2.0328381547999999</v>
       </c>
       <c r="E21" s="1">
-        <v>0.62370062370000001</v>
+        <v>0.83160083159999998</v>
       </c>
       <c r="F21" s="1">
-        <v>2.7767065175000001</v>
+        <v>3.3166216736999998</v>
       </c>
       <c r="G21" s="1">
-        <v>0.96902578299999997</v>
+        <v>1.0036338467000001</v>
       </c>
       <c r="H21" s="1">
-        <v>0.880195599</v>
+        <v>0.97799510999999995</v>
       </c>
       <c r="I21" s="1">
-        <v>1.9170837662</v>
+        <v>2.0681839645000002</v>
       </c>
       <c r="J21" s="1">
-        <v>3.3732501264999999</v>
+        <v>2.9009951088000001</v>
       </c>
       <c r="K21" s="1">
-        <v>3.3891777393</v>
+        <v>3.023300597</v>
       </c>
       <c r="L21" s="1">
-        <v>5.1182910956000001</v>
+        <v>4.6512518183999996</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2931,31 +2943,31 @@
         <v>14</v>
       </c>
       <c r="D22" s="1">
-        <v>4.1438623925</v>
+        <v>4.3002345581999997</v>
       </c>
       <c r="E22" s="1">
-        <v>1.2474012474</v>
+        <v>1.4553014553000001</v>
       </c>
       <c r="F22" s="1">
-        <v>1.8125723101</v>
+        <v>1.8897030467</v>
       </c>
       <c r="G22" s="1">
-        <v>0.84789756009999995</v>
+        <v>4.3606160235000004</v>
       </c>
       <c r="H22" s="1">
-        <v>0.880195599</v>
+        <v>3.5696821515999999</v>
       </c>
       <c r="I22" s="1">
-        <v>0.50051940689999996</v>
+        <v>2.0681839645000002</v>
       </c>
       <c r="J22" s="1">
-        <v>5.0430089390999999</v>
+        <v>7.0163602631000002</v>
       </c>
       <c r="K22" s="1">
-        <v>3.5047178895000002</v>
+        <v>4.8334296168000002</v>
       </c>
       <c r="L22" s="1">
-        <v>1.7686241482</v>
+        <v>3.1352882628000001</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2969,31 +2981,31 @@
         <v>14</v>
       </c>
       <c r="D23" s="1">
-        <v>6.4112587959000003</v>
+        <v>6.4894448787999996</v>
       </c>
       <c r="E23" s="1">
         <v>5.4054054053999998</v>
       </c>
       <c r="F23" s="1">
-        <v>2.2367913613999999</v>
+        <v>2.4296182029</v>
       </c>
       <c r="G23" s="1">
-        <v>2.2322201072999999</v>
+        <v>7.0773490223</v>
       </c>
       <c r="H23" s="1">
-        <v>2.1026894866000001</v>
+        <v>6.4058679707000001</v>
       </c>
       <c r="I23" s="1">
-        <v>0.61384455569999996</v>
+        <v>2.4364906979000001</v>
       </c>
       <c r="J23" s="1">
-        <v>10.963062911</v>
+        <v>10.524540395000001</v>
       </c>
       <c r="K23" s="1">
-        <v>8.5114577316000002</v>
+        <v>8.1263238976000007</v>
       </c>
       <c r="L23" s="1">
-        <v>3.1888829339</v>
+        <v>3.1199754996000002</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -3007,31 +3019,31 @@
         <v>14</v>
       </c>
       <c r="D24" s="1">
-        <v>7.1931196247000004</v>
+        <v>8.4440969507000005</v>
       </c>
       <c r="E24" s="1">
-        <v>5.8212058212000004</v>
+        <v>7.2765072765000003</v>
       </c>
       <c r="F24" s="1">
-        <v>5.1677593521</v>
+        <v>6.2475896645000004</v>
       </c>
       <c r="G24" s="1">
-        <v>1.8515314067999999</v>
+        <v>7.7522062640999998</v>
       </c>
       <c r="H24" s="1">
-        <v>1.5158924204999999</v>
+        <v>6.7970660147000004</v>
       </c>
       <c r="I24" s="1">
-        <v>1.57710832</v>
+        <v>7.3094720937000002</v>
       </c>
       <c r="J24" s="1">
-        <v>7.9777365492000003</v>
+        <v>6.8814302581</v>
       </c>
       <c r="K24" s="1">
-        <v>5.3148469092999999</v>
+        <v>4.9874831504000001</v>
       </c>
       <c r="L24" s="1">
-        <v>4.1344460608000002</v>
+        <v>3.4989663885</v>
       </c>
     </row>
   </sheetData>
@@ -3046,7 +3058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3105,32 +3117,32 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3">
-        <v>0.199837686022797</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="C2" s="4">
+        <v>0.199832219349909</v>
+      </c>
+      <c r="D2" s="4">
         <v>0.23473348671573899</v>
       </c>
-      <c r="E2" s="3">
-        <v>0.378282591856552</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.20845834991290199</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.44623563134333399</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.47789423226328798</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0.57871529449720904</v>
-      </c>
-      <c r="J2" s="3">
-        <v>1.3088684183872701</v>
-      </c>
-      <c r="K2" s="3">
-        <v>1.32386100446903</v>
+      <c r="E2" s="4">
+        <v>0.568624093161466</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.193559472379359</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.84000533555261003</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.60930308762173702</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.42923990021297798</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1.01003629954654</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1.05334994712931</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3140,32 +3152,32 @@
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.25323732263440002</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.334155188892932</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.248995437566537</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.95866648867177795</v>
-      </c>
-      <c r="J3" s="3">
-        <v>1.2558451382217899</v>
-      </c>
-      <c r="K3" s="3">
-        <v>1.57985040808803</v>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.77854969142105301</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1.12004661112502</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.88248874936965005</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1.3387416272313599</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1.49690731751229</v>
+      </c>
+      <c r="K3" s="4">
+        <v>2.0293005894546501</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3175,32 +3187,32 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3">
-        <v>1.76179866169122</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.9082199742750801</v>
-      </c>
-      <c r="E4" s="3">
-        <v>3.7003366931357702</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.88580031240188895</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2.6899415997991198</v>
-      </c>
-      <c r="H4" s="3">
-        <v>2.7409242907527598</v>
-      </c>
-      <c r="I4" s="3">
-        <v>4.0429047441944297</v>
-      </c>
-      <c r="J4" s="3">
-        <v>6.4726341304499</v>
-      </c>
-      <c r="K4" s="3">
-        <v>7.98088482103097</v>
+      <c r="C4" s="4">
+        <v>2.1769781947612001</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.90845677559217</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4.4566849184515203</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.7914897844478499</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4.4660097817851101</v>
+      </c>
+      <c r="H4" s="4">
+        <v>3.9824493203214599</v>
+      </c>
+      <c r="I4" s="4">
+        <v>3.3481870035132699</v>
+      </c>
+      <c r="J4" s="4">
+        <v>5.2676025030870903</v>
+      </c>
+      <c r="K4" s="4">
+        <v>6.9631326485990099</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3210,32 +3222,32 @@
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3">
-        <v>1.27558147659721</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.46942473781654698</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1.58293042830762</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.58336609578406196</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.50189168393316297</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.80663813781050098</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1.8949475804643201</v>
-      </c>
-      <c r="J5" s="3">
-        <v>2.5105009044701498</v>
-      </c>
-      <c r="K5" s="3">
-        <v>3.3777330196617599</v>
+      <c r="C5" s="4">
+        <v>1.1416496900139901</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.23421418815415601</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.7028711779258101</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.720355592372663</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.95093734542454</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.2633299487122001</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1.8165467400203701</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2.7853294543234899</v>
+      </c>
+      <c r="K5" s="4">
+        <v>3.4329391735427102</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3245,32 +3257,32 @@
       <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3">
-        <v>0.333474544552049</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.56959182760508997</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.49367832075386298</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.50293522314499495</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.926842542224664</v>
-      </c>
-      <c r="I6" s="3">
-        <v>1.97740883539269</v>
-      </c>
-      <c r="J6" s="3">
-        <v>2.5756877441396901</v>
-      </c>
-      <c r="K6" s="3">
-        <v>3.7504000424909298</v>
+      <c r="C6" s="4">
+        <v>0.26590420168441897</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.87599335556038604</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.68839393595356102</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.78184128322069801</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1.61646622316778</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1.8662433677736201</v>
+      </c>
+      <c r="J6" s="4">
+        <v>2.4667774477869799</v>
+      </c>
+      <c r="K6" s="4">
+        <v>3.6166155568780001</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3280,32 +3292,32 @@
       <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="C7" s="4">
+        <v>0.333094399080474</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.60622595299520399</v>
+      </c>
+      <c r="F7" s="4">
         <v>0.20823288528171199</v>
       </c>
-      <c r="G7" s="3">
-        <v>0.166859299118016</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.56466924052338696</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.38367371673141898</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.69031266860868501</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0.92297824264946604</v>
+      <c r="G7" s="4">
+        <v>0.27822890258755301</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.641219241200775</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.69085221427402099</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1.21041904856959</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1.54680962741757</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3315,32 +3327,32 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3">
-        <v>6.6426361761388594E-2</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.22691103823750799</v>
-      </c>
-      <c r="F8" s="3">
-        <v>2.6218658680261302</v>
-      </c>
-      <c r="G8" s="3">
-        <v>3.3170439172387698</v>
-      </c>
-      <c r="H8" s="3">
-        <v>5.4127844078581298</v>
-      </c>
-      <c r="I8" s="3">
-        <v>7.0916867247319404</v>
-      </c>
-      <c r="J8" s="3">
-        <v>9.2414914325723796</v>
-      </c>
-      <c r="K8" s="3">
-        <v>12.6649422418553</v>
+      <c r="C8" s="4">
+        <v>1.0707414939875299</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.94263537882487503</v>
+      </c>
+      <c r="E8" s="4">
+        <v>6.3755078125423799</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3.0941940429840198</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4.2133020454954799</v>
+      </c>
+      <c r="H8" s="4">
+        <v>6.7097043671604304</v>
+      </c>
+      <c r="I8" s="4">
+        <v>8.7727157240418396</v>
+      </c>
+      <c r="J8" s="4">
+        <v>11.7405893691617</v>
+      </c>
+      <c r="K8" s="4">
+        <v>15.9136332761502</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3350,32 +3362,32 @@
       <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3">
-        <v>0.87036337775196904</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.1858535223359601</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.45511372131222899</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.31295825264687599</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.66949556419590806</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0.33557409985459202</v>
-      </c>
-      <c r="I9" s="3">
-        <v>1.8159243048781599</v>
-      </c>
-      <c r="J9" s="3">
-        <v>2.0685756854997601</v>
-      </c>
-      <c r="K9" s="3">
-        <v>1.70913803526758</v>
+      <c r="C9" s="4">
+        <v>0.87016878333895697</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.42343091341174</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.53118994443084</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.869781750862202</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1.3493211833641401</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.79445563777636397</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1.7052814988686</v>
+      </c>
+      <c r="J9" s="4">
+        <v>2.1392041949896901</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1.9707752691948599</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3386,31 +3398,31 @@
         <v>25</v>
       </c>
       <c r="C10" s="3">
-        <v>4.61618445972909</v>
+        <v>4.4778606797157403</v>
       </c>
       <c r="D10" s="3">
-        <v>3.1226160726127299</v>
+        <v>3.6124499713076901</v>
       </c>
       <c r="E10" s="3">
-        <v>2.5578898111748898</v>
+        <v>2.9142566259146401</v>
       </c>
       <c r="F10" s="3">
-        <v>2.7719740271384601</v>
+        <v>4.2877074940102302</v>
       </c>
       <c r="G10" s="3">
-        <v>2.4014934485678001</v>
+        <v>3.6400026576387399</v>
       </c>
       <c r="H10" s="3">
-        <v>1.4041482320584999</v>
+        <v>2.32122883725481</v>
       </c>
       <c r="I10" s="3">
-        <v>3.6017388493187998</v>
+        <v>3.5745853115247499</v>
       </c>
       <c r="J10" s="3">
-        <v>3.4433239652162899</v>
+        <v>3.4157761145875498</v>
       </c>
       <c r="K10" s="3">
-        <v>2.25484630890824</v>
+        <v>2.17202272519989</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3421,31 +3433,31 @@
         <v>26</v>
       </c>
       <c r="C11" s="3">
-        <v>2.46390987581636</v>
+        <v>2.3968737285047101</v>
       </c>
       <c r="D11" s="3">
-        <v>0.70625656627314104</v>
+        <v>0.94544748591506</v>
       </c>
       <c r="E11" s="3">
-        <v>1.2676876250303399</v>
+        <v>1.5826343261287701</v>
       </c>
       <c r="F11" s="3">
-        <v>1.51066273528743</v>
+        <v>2.5641464942484502</v>
       </c>
       <c r="G11" s="3">
-        <v>1.4045419097480301</v>
+        <v>2.3931465262600198</v>
       </c>
       <c r="H11" s="3">
-        <v>0.84972261989946196</v>
+        <v>1.6806598221109501</v>
       </c>
       <c r="I11" s="3">
-        <v>2.2132052533405902</v>
+        <v>1.96362322541428</v>
       </c>
       <c r="J11" s="3">
-        <v>2.1985967479991499</v>
+        <v>1.82926600231501</v>
       </c>
       <c r="K11" s="3">
-        <v>1.4943206234175801</v>
+        <v>1.3454657207184899</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3462,10 +3474,10 @@
         <v>0</v>
       </c>
       <c r="E12" s="3">
-        <v>3.7695093394736999E-2</v>
+        <v>0.113117851095447</v>
       </c>
       <c r="F12" s="3">
-        <v>1.48571758633863E-2</v>
+        <v>2.9716201126503399E-2</v>
       </c>
       <c r="G12" s="3">
         <v>0</v>
@@ -3477,10 +3489,10 @@
         <v>5.8846381339530698E-2</v>
       </c>
       <c r="J12" s="3">
-        <v>1.1033123233253001E-2</v>
+        <v>2.2067486330649699E-2</v>
       </c>
       <c r="K12" s="3">
-        <v>5.6022145322827399E-2</v>
+        <v>4.3276841521477101E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3497,25 +3509,25 @@
         <v>0</v>
       </c>
       <c r="E13" s="3">
-        <v>0.113270916742335</v>
+        <v>7.5433549289351101E-2</v>
       </c>
       <c r="F13" s="3">
-        <v>4.4585437824572798E-2</v>
+        <v>0.11892401845893499</v>
       </c>
       <c r="G13" s="3">
-        <v>5.56663887798498E-2</v>
+        <v>0</v>
       </c>
       <c r="H13" s="3">
-        <v>2.1599421649885701E-2</v>
+        <v>7.5619239273229694E-2</v>
       </c>
       <c r="I13" s="3">
-        <v>0.213921795569534</v>
+        <v>0.15476582494164701</v>
       </c>
       <c r="J13" s="3">
-        <v>9.94968331115125E-2</v>
+        <v>0.12152613413010099</v>
       </c>
       <c r="K13" s="3">
-        <v>0.21180450246948801</v>
+        <v>0.14783991263971899</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3526,7 +3538,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="3">
-        <v>0</v>
+        <v>0.133108358041265</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -3535,22 +3547,22 @@
         <v>0</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
+        <v>4.4598467269653802E-2</v>
       </c>
       <c r="G14" s="3">
-        <v>5.55793106500534E-2</v>
+        <v>0.11125274705137</v>
       </c>
       <c r="H14" s="3">
-        <v>4.3217129246641998E-2</v>
+        <v>4.3217359357073298E-2</v>
       </c>
       <c r="I14" s="3">
-        <v>0.15465607485046501</v>
+        <v>0.13990170644387001</v>
       </c>
       <c r="J14" s="3">
-        <v>7.7285674514398897E-2</v>
+        <v>0.121605142480009</v>
       </c>
       <c r="K14" s="3">
-        <v>0.104495754471888</v>
+        <v>7.8974405116236199E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3567,7 +3579,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="3">
-        <v>0</v>
+        <v>3.7699100795415601E-2</v>
       </c>
       <c r="F15" s="3">
         <v>0</v>
@@ -3576,16 +3588,16 @@
         <v>0</v>
       </c>
       <c r="H15" s="3">
-        <v>0</v>
+        <v>1.0799704438432201E-2</v>
       </c>
       <c r="I15" s="3">
         <v>0</v>
       </c>
       <c r="J15" s="3">
-        <v>3.3116946114196001E-2</v>
+        <v>2.2075482132579202E-2</v>
       </c>
       <c r="K15" s="3">
-        <v>1.7808038848618601E-2</v>
+        <v>1.2719141847029301E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3602,25 +3614,25 @@
         <v>0</v>
       </c>
       <c r="E16" s="3">
-        <v>0</v>
+        <v>0.113101855150691</v>
       </c>
       <c r="F16" s="3">
-        <v>4.4581991194593697E-2</v>
+        <v>7.4329356890362103E-2</v>
       </c>
       <c r="G16" s="3">
-        <v>5.5592422686766202E-2</v>
+        <v>0.111243767759112</v>
       </c>
       <c r="H16" s="3">
-        <v>5.40113781010979E-2</v>
+        <v>8.6470477522697403E-2</v>
       </c>
       <c r="I16" s="3">
-        <v>0.31785738932281199</v>
+        <v>0.39258072967534302</v>
       </c>
       <c r="J16" s="3">
-        <v>0.71283157828896504</v>
+        <v>0.848777087084577</v>
       </c>
       <c r="K16" s="3">
-        <v>0.327559402895924</v>
+        <v>0.44387645323584102</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3631,31 +3643,31 @@
         <v>34</v>
       </c>
       <c r="C17" s="3">
-        <v>0.94161386374287204</v>
+        <v>0.80640561667576205</v>
       </c>
       <c r="D17" s="3">
         <v>0</v>
       </c>
       <c r="E17" s="3">
-        <v>1.53014094889717</v>
+        <v>1.8459672375388001</v>
       </c>
       <c r="F17" s="3">
-        <v>0.55356119556179495</v>
+        <v>0.74788809914764698</v>
       </c>
       <c r="G17" s="3">
-        <v>0.61635545273691705</v>
+        <v>0.84100593749575103</v>
       </c>
       <c r="H17" s="3">
-        <v>0.88289958664742696</v>
+        <v>1.27959690567872</v>
       </c>
       <c r="I17" s="3">
-        <v>5.29175742208262</v>
+        <v>1.9909472855188799</v>
       </c>
       <c r="J17" s="3">
-        <v>6.9133031464033996</v>
+        <v>2.48196022669512</v>
       </c>
       <c r="K17" s="3">
-        <v>7.7682158790993103</v>
+        <v>2.4211944754385502</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3672,25 +3684,25 @@
         <v>0</v>
       </c>
       <c r="E18" s="3">
-        <v>7.5432926135706693E-2</v>
+        <v>0.15102023939891801</v>
       </c>
       <c r="F18" s="3">
-        <v>1.4858191226154E-2</v>
+        <v>2.9728681523857999E-2</v>
       </c>
       <c r="G18" s="3">
         <v>5.5563246262028902E-2</v>
       </c>
       <c r="H18" s="3">
-        <v>2.1602027663102201E-2</v>
+        <v>1.0799231857484701E-2</v>
       </c>
       <c r="I18" s="3">
-        <v>8.8318965466400903E-2</v>
+        <v>8.8328434256348995E-2</v>
       </c>
       <c r="J18" s="3">
-        <v>5.5203485867465298E-2</v>
+        <v>1.1033379863308801E-2</v>
       </c>
       <c r="K18" s="3">
-        <v>0.10960832093067201</v>
+        <v>9.1729966902309598E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3707,25 +3719,25 @@
         <v>0</v>
       </c>
       <c r="E19" s="3">
-        <v>0.30229076813176198</v>
+        <v>0.26432640317288097</v>
       </c>
       <c r="F19" s="3">
-        <v>5.9459444060668699E-2</v>
+        <v>0.178409699170266</v>
       </c>
       <c r="G19" s="3">
-        <v>0.16690784462618</v>
+        <v>0.22279934182051001</v>
       </c>
       <c r="H19" s="3">
-        <v>0.11886960926183</v>
+        <v>0.303148152209118</v>
       </c>
       <c r="I19" s="3">
-        <v>0.39231960887858502</v>
+        <v>0.199026718127711</v>
       </c>
       <c r="J19" s="3">
-        <v>0.44489417700380801</v>
+        <v>0.27719711633097199</v>
       </c>
       <c r="K19" s="3">
-        <v>0.66373364357728404</v>
+        <v>0.39981767207990898</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3736,31 +3748,31 @@
         <v>39</v>
       </c>
       <c r="C20" s="3">
-        <v>0.93894256721603297</v>
+        <v>0.87167836983163505</v>
       </c>
       <c r="D20" s="3">
         <v>0.23457971535713401</v>
       </c>
       <c r="E20" s="3">
-        <v>1.5392703584318499</v>
+        <v>1.73432499423454</v>
       </c>
       <c r="F20" s="3">
-        <v>0.37282825626995297</v>
+        <v>0.44750390225569397</v>
       </c>
       <c r="G20" s="3">
-        <v>0.55754931697329502</v>
+        <v>0.72433866390355295</v>
       </c>
       <c r="H20" s="3">
-        <v>1.8290475612963599</v>
+        <v>2.33761772599992</v>
       </c>
       <c r="I20" s="3">
-        <v>2.28581311077162</v>
+        <v>1.73155267528233</v>
       </c>
       <c r="J20" s="3">
-        <v>3.05850466841768</v>
+        <v>2.3519135854594402</v>
       </c>
       <c r="K20" s="3">
-        <v>4.6231991808102499</v>
+        <v>4.0015302825660397</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3771,31 +3783,31 @@
         <v>40</v>
       </c>
       <c r="C21" s="3">
-        <v>1.0039949055684101</v>
+        <v>1.27531190215597</v>
       </c>
       <c r="D21" s="3">
-        <v>0.70515666931054999</v>
+        <v>0.94111735944976704</v>
       </c>
       <c r="E21" s="3">
-        <v>2.7606357837682798</v>
+        <v>3.28658564019505</v>
       </c>
       <c r="F21" s="3">
-        <v>1.16100719905574</v>
+        <v>1.22137472335314</v>
       </c>
       <c r="G21" s="3">
-        <v>1.0651074200819499</v>
+        <v>1.1219974473012</v>
       </c>
       <c r="H21" s="3">
-        <v>1.6032832633988301</v>
+        <v>1.77165389914768</v>
       </c>
       <c r="I21" s="3">
-        <v>2.8631107271485998</v>
+        <v>2.5672618125446802</v>
       </c>
       <c r="J21" s="3">
-        <v>3.49419541812957</v>
+        <v>3.2732168689597301</v>
       </c>
       <c r="K21" s="3">
-        <v>3.85139542118704</v>
+        <v>3.58333856588711</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3806,31 +3818,31 @@
         <v>42</v>
       </c>
       <c r="C22" s="3">
-        <v>3.3645494946850598</v>
+        <v>3.3643976991277702</v>
       </c>
       <c r="D22" s="3">
         <v>0.95254860540341002</v>
       </c>
       <c r="E22" s="3">
-        <v>1.53923143781344</v>
+        <v>1.5791779764702001</v>
       </c>
       <c r="F22" s="3">
-        <v>0.80946179932002005</v>
+        <v>3.4117161995325902</v>
       </c>
       <c r="G22" s="3">
-        <v>0.61258702233310602</v>
+        <v>3.1129277443025698</v>
       </c>
       <c r="H22" s="3">
-        <v>0.37920315945493799</v>
+        <v>1.6678087201937699</v>
       </c>
       <c r="I22" s="3">
-        <v>2.4827384043501102</v>
+        <v>3.5217316641355301</v>
       </c>
       <c r="J22" s="3">
-        <v>1.9542254843192699</v>
+        <v>3.2213043935477401</v>
       </c>
       <c r="K22" s="3">
-        <v>1.11881673019318</v>
+        <v>1.9206388310503</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3841,31 +3853,31 @@
         <v>43</v>
       </c>
       <c r="C23" s="3">
-        <v>5.13292778018441</v>
+        <v>5.1296986045486497</v>
       </c>
       <c r="D23" s="3">
-        <v>5.1336925238698097</v>
+        <v>5.1346891505937098</v>
       </c>
       <c r="E23" s="3">
-        <v>1.6462101241651801</v>
+        <v>1.80350473548023</v>
       </c>
       <c r="F23" s="3">
-        <v>1.69512876314428</v>
+        <v>5.1968411714934399</v>
       </c>
       <c r="G23" s="3">
-        <v>1.9156458681611599</v>
+        <v>6.3875794992928903</v>
       </c>
       <c r="H23" s="3">
-        <v>0.50998794156819705</v>
+        <v>1.88791682743921</v>
       </c>
       <c r="I23" s="3">
-        <v>5.02581853014535</v>
+        <v>4.5802669542494696</v>
       </c>
       <c r="J23" s="3">
-        <v>4.26648271557612</v>
+        <v>3.96984772542935</v>
       </c>
       <c r="K23" s="3">
-        <v>1.6859741939100601</v>
+        <v>1.61963304547565</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3876,37 +3888,38 @@
         <v>44</v>
       </c>
       <c r="C24" s="3">
-        <v>4.3578705504282302</v>
+        <v>4.9506340411815204</v>
       </c>
       <c r="D24" s="3">
-        <v>5.2184251346544004</v>
+        <v>6.5494006814312797</v>
       </c>
       <c r="E24" s="3">
-        <v>3.87079297489367</v>
+        <v>4.8590180879910303</v>
       </c>
       <c r="F24" s="3">
-        <v>0.87052016707761803</v>
+        <v>5.5916124074261697</v>
       </c>
       <c r="G24" s="3">
-        <v>1.1766533204524701</v>
+        <v>6.5726537883388803</v>
       </c>
       <c r="H24" s="3">
-        <v>0.75042587333091004</v>
+        <v>5.7568108157590201</v>
       </c>
       <c r="I24" s="3">
-        <v>4.1105495219205803</v>
+        <v>3.6850793054761901</v>
       </c>
       <c r="J24" s="3">
-        <v>3.1441706011939798</v>
+        <v>2.7617160593643102</v>
       </c>
       <c r="K24" s="3">
-        <v>2.4526474333583601</v>
+        <v>2.0773834163729701</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Postprocess and update Excel and Word documents
Summary of changes since call20170908
* Fixed denominator used in overall prevalence calculation
* Fixed filtering of claims to satisfy physician-diagnosed criterion
  * Use enc_type in ("IP", "AV", "ED", "NH", "HH") instead of provider type
* Fixed incident MI outcome to require inpatient admission of at least 1 day
* In progress incidence rates are greyed-out
</commit_message>
<xml_diff>
--- a/data/processed/tables.xlsx
+++ b/data/processed/tables.xlsx
@@ -181,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +319,12 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -665,7 +671,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -677,6 +683,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3058,7 +3067,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:K7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3222,31 +3233,31 @@
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>1.1416496900139901</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>0.23421418815415601</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>1.7028711779258101</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>0.720355592372663</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="5">
         <v>0.95093734542454</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="5">
         <v>1.2633299487122001</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="5">
         <v>1.8165467400203701</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="5">
         <v>2.7853294543234899</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="5">
         <v>3.4329391735427102</v>
       </c>
     </row>
@@ -3257,31 +3268,31 @@
       <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>0.26590420168441897</v>
       </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
         <v>0.87599335556038604</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <v>0.68839393595356102</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="5">
         <v>0.78184128322069801</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="5">
         <v>1.61646622316778</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="5">
         <v>1.8662433677736201</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="5">
         <v>2.4667774477869799</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="5">
         <v>3.6166155568780001</v>
       </c>
     </row>
@@ -3292,32 +3303,32 @@
       <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>0.333094399080474</v>
       </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
         <v>0.60622595299520399</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="5">
         <v>0.20823288528171199</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="5">
         <v>0.27822890258755301</v>
       </c>
-      <c r="H7" s="4">
-        <v>0.641219241200775</v>
-      </c>
-      <c r="I7" s="4">
+      <c r="H7" s="5">
+        <v>0.630349805535103</v>
+      </c>
+      <c r="I7" s="5">
         <v>0.69085221427402099</v>
       </c>
-      <c r="J7" s="4">
-        <v>1.21041904856959</v>
-      </c>
-      <c r="K7" s="4">
-        <v>1.54680962741757</v>
+      <c r="J7" s="5">
+        <v>1.1992114647865399</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1.52860557927139</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>